<commit_message>
Add archival containers to description sheet.
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/template_bad_description/openn_metadata.xlsx
+++ b/openn/tests/data/sheets/template_bad_description/openn_metadata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30500" windowHeight="19140"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3908" uniqueCount="3739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3916" uniqueCount="3743">
   <si>
     <t>1r</t>
   </si>
@@ -11276,6 +11276,18 @@
   </si>
   <si>
     <t>1909</t>
+  </si>
+  <si>
+    <t>Archival Drawer</t>
+  </si>
+  <si>
+    <t>Archival Box</t>
+  </si>
+  <si>
+    <t>Archival Folder</t>
+  </si>
+  <si>
+    <t>Archival Item</t>
   </si>
 </sst>
 </file>
@@ -11836,13 +11848,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V62"/>
+  <dimension ref="A1:V66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12275,7 +12287,7 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="4" t="s">
-        <v>3729</v>
+        <v>3739</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>2664</v>
@@ -12303,10 +12315,10 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="4" t="s">
-        <v>3730</v>
+        <v>3740</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>3657</v>
+        <v>2664</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="10"/>
@@ -12331,18 +12343,35 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="4" t="s">
-        <v>2661</v>
+        <v>3741</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>2656</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>3726</v>
-      </c>
+        <v>2664</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="4" t="s">
-        <v>3669</v>
+        <v>3742</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>2664</v>
@@ -12370,416 +12399,427 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="4" t="s">
-        <v>2662</v>
+        <v>3729</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>2656</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>3712</v>
-      </c>
+        <v>2664</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="4" t="s">
-        <v>2663</v>
+        <v>3730</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>2664</v>
+        <v>3657</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="A26" s="4" t="s">
+        <v>2661</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>2656</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>3726</v>
       </c>
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="4" t="s">
-        <v>2680</v>
+        <v>3669</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="4" t="s">
-        <v>2681</v>
+        <v>2662</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>2664</v>
-      </c>
-      <c r="C28" s="19">
-        <v>1903</v>
-      </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="11"/>
-      <c r="T28" s="11"/>
-      <c r="U28" s="11"/>
-      <c r="V28" s="11"/>
+        <v>2656</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>3712</v>
+      </c>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="4" t="s">
-        <v>2682</v>
+        <v>2663</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C29" s="22" t="s">
-        <v>3738</v>
-      </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="11"/>
-      <c r="S29" s="11"/>
-      <c r="T29" s="11"/>
-      <c r="U29" s="11"/>
-      <c r="V29" s="11"/>
-    </row>
-    <row r="30" spans="1:22">
-      <c r="A30" s="4" t="s">
-        <v>3731</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>2664</v>
-      </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="11"/>
-      <c r="U30" s="11"/>
-      <c r="V30" s="11"/>
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="4" t="s">
-        <v>3732</v>
+        <v>2680</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>2656</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>3737</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>2664</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+    </row>
+    <row r="32" spans="1:22">
+      <c r="A32" s="4" t="s">
+        <v>2681</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C32" s="19">
+        <v>1903</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+    </row>
+    <row r="33" spans="1:22">
       <c r="A33" s="4" t="s">
-        <v>2665</v>
+        <v>2682</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>3727</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="C33" s="22" t="s">
+        <v>3738</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="11"/>
+    </row>
+    <row r="34" spans="1:22">
       <c r="A34" s="4" t="s">
-        <v>2666</v>
+        <v>3731</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+    </row>
+    <row r="35" spans="1:22">
+      <c r="A35" s="4" t="s">
+        <v>3732</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>2656</v>
       </c>
-      <c r="C34" s="17"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="4" t="s">
-        <v>3733</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>2664</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="C35" s="20" t="s">
+        <v>3737</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22">
       <c r="A37" s="4" t="s">
-        <v>3734</v>
+        <v>2665</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>2664</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="C37" s="17" t="s">
+        <v>3727</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22">
       <c r="A38" s="4" t="s">
-        <v>3735</v>
+        <v>2666</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>2656</v>
+      </c>
+      <c r="C38" s="17"/>
+    </row>
+    <row r="40" spans="1:22">
+      <c r="A40" s="4" t="s">
+        <v>3733</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>2664</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="4" t="s">
-        <v>3736</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>2664</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:22">
       <c r="A41" s="4" t="s">
-        <v>2678</v>
+        <v>3734</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C41" s="17"/>
-    </row>
-    <row r="42" spans="1:7">
+    </row>
+    <row r="42" spans="1:22">
       <c r="A42" s="4" t="s">
-        <v>2679</v>
+        <v>3735</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>2664</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="4" t="s">
-        <v>2668</v>
-      </c>
-      <c r="B44" s="5" t="s">
+    <row r="43" spans="1:22">
+      <c r="A43" s="4" t="s">
+        <v>3736</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-    </row>
-    <row r="45" spans="1:7">
+    </row>
+    <row r="45" spans="1:22">
       <c r="A45" s="4" t="s">
-        <v>3670</v>
+        <v>2678</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>2664</v>
       </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="4" t="s">
-        <v>2669</v>
-      </c>
-      <c r="B47" s="5" t="s">
+      <c r="C45" s="17"/>
+    </row>
+    <row r="46" spans="1:22">
+      <c r="A46" s="4" t="s">
+        <v>2679</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C47" s="17" t="s">
-        <v>3679</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>3705</v>
-      </c>
-      <c r="E47" s="17" t="s">
-        <v>3706</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>3707</v>
-      </c>
-      <c r="G47" s="17"/>
-    </row>
-    <row r="48" spans="1:7">
+    </row>
+    <row r="48" spans="1:22">
       <c r="A48" s="4" t="s">
-        <v>3671</v>
+        <v>2668</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>3708</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>3709</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>3710</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>3711</v>
-      </c>
-    </row>
-    <row r="50" spans="1:22">
-      <c r="A50" s="4" t="s">
-        <v>2670</v>
-      </c>
-      <c r="B50" s="5" t="s">
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+    </row>
+    <row r="49" spans="1:22">
+      <c r="A49" s="4" t="s">
+        <v>3670</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>2664</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>3680</v>
       </c>
     </row>
     <row r="51" spans="1:22">
       <c r="A51" s="4" t="s">
-        <v>3672</v>
+        <v>2669</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C51" s="6" t="s">
-        <v>3681</v>
-      </c>
-    </row>
-    <row r="53" spans="1:22">
-      <c r="A53" s="4" t="s">
-        <v>2671</v>
-      </c>
-      <c r="B53" s="5" t="s">
+      <c r="C51" s="17" t="s">
+        <v>3679</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>3705</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>3706</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>3707</v>
+      </c>
+      <c r="G51" s="17"/>
+    </row>
+    <row r="52" spans="1:22">
+      <c r="A52" s="4" t="s">
+        <v>3671</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C53" s="17" t="s">
-        <v>3682</v>
+      <c r="C52" s="6" t="s">
+        <v>3708</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>3709</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>3710</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>3711</v>
       </c>
     </row>
     <row r="54" spans="1:22">
       <c r="A54" s="4" t="s">
-        <v>3673</v>
+        <v>2670</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C54" s="18" t="s">
-        <v>3683</v>
-      </c>
-    </row>
-    <row r="56" spans="1:22">
-      <c r="A56" s="4" t="s">
-        <v>3661</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>2656</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>2672</v>
-      </c>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="11"/>
-      <c r="L56" s="11"/>
-      <c r="M56" s="11"/>
-      <c r="N56" s="11"/>
-      <c r="O56" s="11"/>
-      <c r="P56" s="11"/>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="11"/>
-      <c r="S56" s="11"/>
-      <c r="T56" s="11"/>
-      <c r="U56" s="11"/>
-      <c r="V56" s="11"/>
+      <c r="C54" s="17" t="s">
+        <v>3680</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22">
+      <c r="A55" s="4" t="s">
+        <v>3672</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>3681</v>
+      </c>
     </row>
     <row r="57" spans="1:22">
       <c r="A57" s="4" t="s">
-        <v>3656</v>
+        <v>2671</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>3657</v>
-      </c>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="11"/>
-      <c r="K57" s="11"/>
-      <c r="L57" s="11"/>
-      <c r="M57" s="11"/>
-      <c r="N57" s="11"/>
-      <c r="O57" s="11"/>
-      <c r="P57" s="11"/>
-      <c r="Q57" s="11"/>
-      <c r="R57" s="11"/>
-      <c r="S57" s="11"/>
-      <c r="T57" s="11"/>
-      <c r="U57" s="11"/>
-      <c r="V57" s="11"/>
+        <v>2664</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>3682</v>
+      </c>
     </row>
     <row r="58" spans="1:22">
       <c r="A58" s="4" t="s">
-        <v>3658</v>
+        <v>3673</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>3657</v>
-      </c>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-      <c r="L58" s="11"/>
-      <c r="M58" s="11"/>
-      <c r="N58" s="11"/>
-      <c r="O58" s="11"/>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="11"/>
-      <c r="R58" s="11"/>
-      <c r="S58" s="11"/>
-      <c r="T58" s="11"/>
-      <c r="U58" s="11"/>
-      <c r="V58" s="11"/>
+        <v>2664</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>3683</v>
+      </c>
     </row>
     <row r="60" spans="1:22">
       <c r="A60" s="4" t="s">
-        <v>3662</v>
+        <v>3661</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>2656</v>
       </c>
-      <c r="C60" s="21" t="s">
-        <v>2674</v>
+      <c r="C60" s="17" t="s">
+        <v>2672</v>
       </c>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
@@ -12803,13 +12843,10 @@
     </row>
     <row r="61" spans="1:22">
       <c r="A61" s="4" t="s">
-        <v>3659</v>
+        <v>3656</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>3657</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>3684</v>
       </c>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
@@ -12833,13 +12870,10 @@
     </row>
     <row r="62" spans="1:22">
       <c r="A62" s="4" t="s">
-        <v>3660</v>
+        <v>3658</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>3657</v>
-      </c>
-      <c r="C62" s="6">
-        <v>2012</v>
       </c>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
@@ -12861,15 +12895,105 @@
       <c r="U62" s="11"/>
       <c r="V62" s="11"/>
     </row>
+    <row r="64" spans="1:22">
+      <c r="A64" s="4" t="s">
+        <v>3662</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>2656</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>2674</v>
+      </c>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="11"/>
+      <c r="O64" s="11"/>
+      <c r="P64" s="11"/>
+      <c r="Q64" s="11"/>
+      <c r="R64" s="11"/>
+      <c r="S64" s="11"/>
+      <c r="T64" s="11"/>
+      <c r="U64" s="11"/>
+      <c r="V64" s="11"/>
+    </row>
+    <row r="65" spans="1:22">
+      <c r="A65" s="4" t="s">
+        <v>3659</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>3657</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>3684</v>
+      </c>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="11"/>
+      <c r="L65" s="11"/>
+      <c r="M65" s="11"/>
+      <c r="N65" s="11"/>
+      <c r="O65" s="11"/>
+      <c r="P65" s="11"/>
+      <c r="Q65" s="11"/>
+      <c r="R65" s="11"/>
+      <c r="S65" s="11"/>
+      <c r="T65" s="11"/>
+      <c r="U65" s="11"/>
+      <c r="V65" s="11"/>
+    </row>
+    <row r="66" spans="1:22">
+      <c r="A66" s="4" t="s">
+        <v>3660</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>3657</v>
+      </c>
+      <c r="C66" s="6">
+        <v>2012</v>
+      </c>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="11"/>
+      <c r="L66" s="11"/>
+      <c r="M66" s="11"/>
+      <c r="N66" s="11"/>
+      <c r="O66" s="11"/>
+      <c r="P66" s="11"/>
+      <c r="Q66" s="11"/>
+      <c r="R66" s="11"/>
+      <c r="S66" s="11"/>
+      <c r="T66" s="11"/>
+      <c r="U66" s="11"/>
+      <c r="V66" s="11"/>
+    </row>
   </sheetData>
-  <dataValidations xWindow="298" yWindow="489" count="29">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Source URL" prompt="[Optional; multiple values]_x000d__x000d_URL for a finding aid or catalog record for the manuscript." sqref="C42"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Language" prompt="[Required; multiple values]_x000d__x000d_One or more language codes for the manuscript content. Use ISO-539-2 http://www.loc.gov/standards/iso639-2/php/code_list.php. Use bibliographic code rather than terminology code when applicable. " sqref="C34"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="[Optional; single value]_x000d__x000d_From 520 and 545 of catalog record; or biog/hist and scope and contents notes of finding aids. Suggested limit: 1000 words for both 520 and 545 notes combined." sqref="C33"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Date" prompt="[Required; one value per field]_x000d__x000d_Date or dates of mansucript creation. A single year, 'Date when' , or a range expressed by two years, 'Date start' and 'Date end'." sqref="C27"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Creator URI" prompt="[Optional; multiple values]_x000d__x000d_If available, URI to authority record for the above named author (e.g., VIAF or LCNAF)." sqref="C25:C26"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Creator name" prompt="[Required; multiple values]_x000d__x000d_Either (1) the name(s) of manuscript's author(s), (2) Anonymous, or (3) Unknown. When an author name cannot be given, use 'Anonymous' for authors who intentionally do not reveal identity and 'Unknown' otherwise." sqref="C24"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Title" prompt="[Required; multiple values]_x000d__x000d_A title for the manuscript, either a formal title or one devised for the manuscript. Ideally, title should conform with the recommendation in DACS (Describing Archives: A Content Standard). Alternate titles may be provided. " sqref="C22"/>
+  <dataValidations xWindow="298" yWindow="489" count="33">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Source URL" prompt="[Optional; multiple values]_x000d__x000d_URL for a finding aid or catalog record for the manuscript." sqref="C46"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Language" prompt="[Required; multiple values]_x000d__x000d_One or more language codes for the manuscript content. Use ISO-539-2 http://www.loc.gov/standards/iso639-2/php/code_list.php. Use bibliographic code rather than terminology code when applicable. " sqref="C38"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="[Optional; single value]_x000d__x000d_From 520 and 545 of catalog record; or biog/hist and scope and contents notes of finding aids. Suggested limit: 1000 words for both 520 and 545 notes combined." sqref="C37"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Date" prompt="[Required; one value per field]_x000d__x000d_Date or dates of mansucript creation. A single year, 'Date when' , or a range expressed by two years, 'Date start' and 'Date end'." sqref="C31"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Creator URI" prompt="[Optional; multiple values]_x000d__x000d_If available, URI to authority record for the above named author (e.g., VIAF or LCNAF)." sqref="C29:C30"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Creator name" prompt="[Required; multiple values]_x000d__x000d_Either (1) the name(s) of manuscript's author(s), (2) Anonymous, or (3) Unknown. When an author name cannot be given, use 'Anonymous' for authors who intentionally do not reveal identity and 'Unknown' otherwise." sqref="C28"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Title" prompt="[Required; multiple values]_x000d__x000d_A title for the manuscript, either a formal title or one devised for the manuscript. Ideally, title should conform with the recommendation in DACS (Describing Archives: A Content Standard). Alternate titles may be provided. " sqref="C26"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Repository name" prompt="[Required; multiple values]_x000d__x000d_Manuscript identifier, like call number. List primary identifier first. " sqref="C19"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Repository name" prompt="[Required; single value]_x000d__x000d_Repository where the manuscript is kept. " sqref="C17"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Repository City" prompt="[Required; single value]_x000d__x000d_City of the repository where the manuscript is kept. " sqref="C16"/>
@@ -12877,35 +13001,39 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata creator" prompt="The individual or organization responsible for the creation of this metadata record. One name per column." sqref="C14"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Administrative contact" prompt="[Required; multiple values]_x000d__x000d_Person or persons to contact with problems or questions about this metadata of these files during processing._x000d__x000d_THIS VALUE IS NOT FOR PUBLICATION." sqref="C8"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Administrative contact email" prompt="[Required; multiple values]_x000d__x000d_Email address of the above-named person._x000d__x000d_THIS VALUE IS NOT FOR PUBLICATION." sqref="C9"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright holder" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Image rights&quot; is CC0 or CC-BY._x000d__x000d_Copyright does not apply to public domain material._x000d_ _x000d_" sqref="C57"/>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright year" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Image rights&quot; is CC0 or CC-BY. _x000d__x000d_Copyright does not apply to public domain material._x000d__x000d_The year of the images' copyright. Current year will be used by default if &quot;Image rights&quot; is CC0 or CC-BY._x000d_" sqref="C58">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright holder" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Image rights&quot; is CC0 or CC-BY._x000d__x000d_Copyright does not apply to public domain material._x000d_ _x000d_" sqref="C61"/>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright year" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Image rights&quot; is CC0 or CC-BY. _x000d__x000d_Copyright does not apply to public domain material._x000d__x000d_The year of the images' copyright. Current year will be used by default if &quot;Image rights&quot; is CC0 or CC-BY._x000d_" sqref="C62">
       <formula1>1800</formula1>
       <formula2>2100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright holder" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Metadata rights&quot; is CC0 or CC-BY._x000d__x000d_Copyright does not apply to public domain material._x000d_ _x000d_" sqref="C61"/>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright year" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Metadata rights&quot; is CC0 or CC-BY.  Copyright does not apply to public domain material._x000d__x000d_The year of the metadata's copyright. Current year will be used by default if &quot;Metada rights&quot; is CC0 or CC-BY." sqref="C62">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright holder" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Metadata rights&quot; is CC0 or CC-BY._x000d__x000d_Copyright does not apply to public domain material._x000d_ _x000d_" sqref="C65"/>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright year" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Metadata rights&quot; is CC0 or CC-BY.  Copyright does not apply to public domain material._x000d__x000d_The year of the metadata's copyright. Current year will be used by default if &quot;Metada rights&quot; is CC0 or CC-BY." sqref="C66">
       <formula1>1800</formula1>
       <formula2>2100</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter PACSCL Diaires Project ID" prompt="[required; single value]_x000d__x000d_This is the number that was provided to you for this diary, a number like 'PDP001', 'PDP002', etc." sqref="C12"/>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter Volume number" prompt="[reqiued for multi-volume objects; single value]_x000d__x000d_If a multi-volume work, enter a whole number volume here. This value is used for database sorting._x000d__x000d_Complex or non-numeric volume numbers, like 'Volume A' or 'Vol. IV', should be added to the volume title." sqref="C23">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter Volume number" prompt="[reqiued for multi-volume objects; single value]_x000d__x000d_If a multi-volume work, enter a whole number volume here. This value is used for database sorting._x000d__x000d_Complex or non-numeric volume numbers, like 'Volume A' or 'Vol. IV', should be added to the volume title." sqref="C27">
       <formula1>1</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Source" prompt="[Optional; multiple value]_x000d__x000d_Name of a larger collection to which this manuscript belongs." sqref="C18 C35 C40:C41"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Alternate ID" prompt="[Optional; single value]_x000d__x000d_In addition to a call number, one alternate identifier may be given. This can be an internal control number or URN, such as DOI, PURL, or ARK._x000d__x000d_An ID that is part of a persistent URL should be given in URL form." sqref="C20"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Alternate ID Type" prompt="[required if alternate ID provided; single value]_x000d__x000d_The type of Alternate ID above, if entered; e.g., DOI, ARK, PURL, or BibID." sqref="C21"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Date (narrative)" prompt="[Optional; single value]_x000d__x000d_Text description of date of origin for document. If blank, narrative will be built from year values._x000d__x000d_Examples: &quot;Late 19th C.&quot;; &quot;May 3, 1902 to January 26, 1914&quot;; &quot;Main text written in 1872, with annotations added in 1940&quot;" sqref="C30"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Place of origin" prompt="[Required; multiple values]_x000d__x000d_One or more places of origin for this document; if not known, use &quot;Unknown&quot;. Historical or modern place names may be used." sqref="C31"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Bound dimensions" prompt="[Optional; single value]_x000d__x000d_Height and width of the bound document in millimeters._x000d__x000d_Example: &quot;215 x 162 mm&quot;" sqref="C39"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Page dimensions" prompt="[Optional; single value]_x000d__x000d_Height and width of a document page in millimeters._x000d__x000d_Example: &quot;205 x 150 mm&quot;" sqref="C38"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Gaps" prompt="[Optional; single value]_x000d__x000d_Description of pages not imaged or physical pages missing from the document itself. _x000d__x000d_Example: &quot;Blank pages 230-250 were not imaged&quot;; &quot;Folio 23 missing from manuscript.&quot;" sqref="C37"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Number of physical pages" prompt="[Optional; single value]_x000d__x000d_Text describing the number of pages in this document. " sqref="C36"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Source" prompt="[Optional; multiple value]_x000d__x000d_Name of a larger collection to which this manuscript belongs." sqref="C18 C39 C44:C45"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Alternate ID" prompt="[Optional; single value]_x000d__x000d_In addition to a call number, one alternate identifier may be given. This can be an internal control number or URN, such as DOI, PURL, or ARK._x000d__x000d_An ID that is part of a persistent URL should be given in URL form." sqref="C24"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Alternate ID Type" prompt="[required if alternate ID provided; single value]_x000d__x000d_The type of Alternate ID above, if entered; e.g., DOI, ARK, PURL, or BibID." sqref="C25"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Date (narrative)" prompt="[Optional; single value]_x000d__x000d_Text description of date of origin for document. If blank, narrative will be built from year values._x000d__x000d_Examples: &quot;Late 19th C.&quot;; &quot;May 3, 1902 to January 26, 1914&quot;; &quot;Main text written in 1872, with annotations added in 1940&quot;" sqref="C34"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Place of origin" prompt="[Required; multiple values]_x000d__x000d_One or more places of origin for this document; if not known, use &quot;Unknown&quot;. Historical or modern place names may be used." sqref="C35"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Bound dimensions" prompt="[Optional; single value]_x000d__x000d_Height and width of the bound document in millimeters._x000d__x000d_Example: &quot;215 x 162 mm&quot;" sqref="C43"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Page dimensions" prompt="[Optional; single value]_x000d__x000d_Height and width of a document page in millimeters._x000d__x000d_Example: &quot;205 x 150 mm&quot;" sqref="C42"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Gaps" prompt="[Optional; single value]_x000d__x000d_Description of pages not imaged or physical pages missing from the document itself. _x000d__x000d_Example: &quot;Blank pages 230-250 were not imaged&quot;; &quot;Folio 23 missing from manuscript.&quot;" sqref="C41"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Number of physical pages" prompt="[Optional; single value]_x000d__x000d_Text describing the number of pages in this document. " sqref="C40"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Item" prompt="[Optional; single]_x000d__x000d_For archival materials, the item number of this object relative to the given collection, call number, drawer, box, and/or folder. Do not provide if there is only one item in the parent container. _x000d__x000d_Example: &quot;1&quot;, &quot;300&quot;." sqref="C23"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Folder" prompt="[Optional; single]_x000d__x000d_For archival materials, the folder number of this object relative to the given collection, call number, drawer, and/or box. Do not provide if there is only one item in the parent container. _x000d__x000d_Example: &quot;1&quot;, &quot;300&quot;." sqref="C22"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Box" prompt="[Optional; single]_x000d__x000d_For archival materials, the box number of this object relative to the given collection, and/or call number. Do not provide if there is only one item in the parent container. _x000d__x000d_Example: &quot;1&quot;, &quot;300&quot;." sqref="C21"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Drawer" prompt="[Optional; single]_x000d__x000d_For archival materials, the drawer number of this object relative to the given collection and/or call number. _x000d__x000d_Example: &quot;1&quot;, &quot;300&quot;." sqref="C20"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C9" r:id="rId1"/>
     <hyperlink ref="C15" r:id="rId2"/>
-    <hyperlink ref="C54" r:id="rId3"/>
+    <hyperlink ref="C58" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -12916,13 +13044,13 @@
           <x14:formula1>
             <xm:f>'VALUE LISTS'!$D$3:$D$12</xm:f>
           </x14:formula1>
-          <xm:sqref>C56</xm:sqref>
+          <xm:sqref>C60</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select metadata licence" prompt="[Required; single value]_x000d__x000d_PD - metadata in Public Domain_x000d__x000d_CC0 - &quot;CC zero&quot;; metadata copyrighted but released to Public Domain_x000d__x000d_CC-BY - metadata released with Creative Commons Attribution License">
           <x14:formula1>
             <xm:f>'VALUE LISTS'!$D$3:$D$12</xm:f>
           </x14:formula1>
-          <xm:sqref>C60</xm:sqref>
+          <xm:sqref>C64</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>